<commit_message>
some more progress on my term paper
</commit_message>
<xml_diff>
--- a/descreteMath/termpaper1/курсачтаблица.xlsx
+++ b/descreteMath/termpaper1/курсачтаблица.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernie\Documents\GitHub\ITMO-Labs\descreteMath\termpaper1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\ITMO-Labs\descreteMath\termpaper1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC88A920-34E6-4F25-AA48-7D91D27BA4E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4A1638-923E-44CE-BD8B-47EA95424380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21510" yWindow="2235" windowWidth="13530" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2592" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,7 +373,172 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -680,21 +845,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F17" sqref="B17:F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
-    <col min="2" max="6" width="3.28515625" customWidth="1"/>
+    <col min="1" max="1" width="3.88671875" customWidth="1"/>
+    <col min="2" max="6" width="3.33203125" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="10" max="10" width="3.42578125" customWidth="1"/>
+    <col min="10" max="10" width="3.44140625" customWidth="1"/>
+    <col min="11" max="11" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -726,7 +892,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -766,29 +932,33 @@
         <f>IF(I2 = 7, "d", IF(AND(G2 + H2 &gt;= 5, G2 + H2 &lt; 9), 1, 0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" t="str">
+        <f>IF(J2 &lt;&gt;0, SUM(B2:F2), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>1</v>
       </c>
       <c r="B3" s="4">
-        <f t="shared" ref="B3:B34" si="0">IF($A3 - 16 &gt;= 0, 1, 0)</f>
+        <f t="shared" ref="B3:B33" si="0">IF($A3 - 16 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C34" si="1">IF($A3 - 16 * $B3 - 8 &gt;= 0, 1, 0)</f>
+        <f t="shared" ref="C3:C33" si="1">IF($A3 - 16 * $B3 - 8 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="D3" s="4">
-        <f t="shared" ref="D3:D34" si="2">IF($A3 - 16 * $B3 - 8 * $C3 - 4 &gt;= 0, 1, 0)</f>
+        <f t="shared" ref="D3:D33" si="2">IF($A3 - 16 * $B3 - 8 * $C3 - 4 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E34" si="3">IF($A3 - 16 * $B3 - 8 * $C3 - 4 * $D3 - 2 &gt;= 0, 1, 0)</f>
+        <f t="shared" ref="E3:E33" si="3">IF($A3 - 16 * $B3 - 8 * $C3 - 4 * $D3 - 2 &gt;= 0, 1, 0)</f>
         <v>0</v>
       </c>
       <c r="F3" s="4">
-        <f t="shared" ref="F3:F34" si="4">IF($A3 - 16 * $B3 - 8 * $C3 - 4 * $D3 - 2 * $E3 - 1 &gt;= 0, 1, 0)</f>
+        <f t="shared" ref="F3:F33" si="4">IF($A3 - 16 * $B3 - 8 * $C3 - 4 * $D3 - 2 * $E3 - 1 &gt;= 0, 1, 0)</f>
         <v>1</v>
       </c>
       <c r="G3" s="4">
@@ -807,8 +977,12 @@
         <f t="shared" ref="J3:J18" si="8">IF(I3 = 7, "d", IF(AND(G3 + H3 &gt;= 5, G3 + H3 &lt; 9), 1, 0))</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" t="str">
+        <f t="shared" ref="K3:K33" si="9">IF(J3 &lt;&gt;0, SUM(B3:F3), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -848,8 +1022,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -889,8 +1067,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K5" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -930,8 +1112,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -971,8 +1157,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K7" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1012,8 +1202,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1053,8 +1247,12 @@
         <f t="shared" si="8"/>
         <v>d</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1094,8 +1292,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1135,8 +1337,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1176,8 +1382,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1217,8 +1427,12 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1258,8 +1472,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1299,8 +1517,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K15" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1340,8 +1562,12 @@
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1381,8 +1607,12 @@
         <f t="shared" si="8"/>
         <v>d</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1422,8 +1652,12 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K18" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1448,23 +1682,27 @@
         <v>1</v>
       </c>
       <c r="G19" s="4">
-        <f t="shared" ref="G19:G34" si="9">D19 + (C19 * 2) + (B19 * 4)</f>
+        <f t="shared" ref="G19:G33" si="10">D19 + (C19 * 2) + (B19 * 4)</f>
         <v>4</v>
       </c>
       <c r="H19" s="4">
-        <f t="shared" ref="H19:H34" si="10">F19 + (E19 * 2)</f>
+        <f t="shared" ref="H19:H33" si="11">F19 + (E19 * 2)</f>
         <v>1</v>
       </c>
       <c r="I19" s="4">
-        <f t="shared" ref="I19:I34" si="11">F19 + (E19 * 2) + (D19 * 4)</f>
+        <f t="shared" ref="I19:I33" si="12">F19 + (E19 * 2) + (D19 * 4)</f>
         <v>1</v>
       </c>
       <c r="J19" s="4">
-        <f t="shared" ref="J19:J34" si="12">IF(I19 = 7, "d", IF(AND(G19 + H19 &gt;= 5, G19 + H19 &lt; 9), 1, 0))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J19:J33" si="13">IF(I19 = 7, "d", IF(AND(G19 + H19 &gt;= 5, G19 + H19 &lt; 9), 1, 0))</f>
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1489,23 +1727,27 @@
         <v>0</v>
       </c>
       <c r="G20" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="H20" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="I20" s="4">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
+      <c r="I20" s="4">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
       <c r="J20" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1530,23 +1772,27 @@
         <v>1</v>
       </c>
       <c r="G21" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
       <c r="H21" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I21" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="J21" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -1571,23 +1817,27 @@
         <v>0</v>
       </c>
       <c r="G22" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="H22" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I22" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="J22" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -1612,23 +1862,27 @@
         <v>1</v>
       </c>
       <c r="G23" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="H23" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="I23" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="J23" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -1653,23 +1907,27 @@
         <v>0</v>
       </c>
       <c r="G24" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="H24" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="I24" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="J24" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -1694,23 +1952,27 @@
         <v>1</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>5</v>
       </c>
       <c r="H25" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I25" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="J25" s="4" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>d</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -1735,23 +1997,27 @@
         <v>0</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <f t="shared" si="9"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -1776,23 +2042,27 @@
         <v>1</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="I27" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="J27" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -1817,23 +2087,27 @@
         <v>0</v>
       </c>
       <c r="G28" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="H28" s="4">
-        <f t="shared" si="10"/>
-        <v>2</v>
-      </c>
-      <c r="I28" s="4">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
+      <c r="I28" s="4">
+        <f t="shared" si="12"/>
+        <v>2</v>
+      </c>
       <c r="J28" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -1858,23 +2132,27 @@
         <v>1</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I29" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>3</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -1899,23 +2177,27 @@
         <v>0</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="I30" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="9"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -1940,23 +2222,27 @@
         <v>1</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="I31" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>5</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="9"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -1981,23 +2267,27 @@
         <v>0</v>
       </c>
       <c r="G32" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="H32" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="I32" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>6</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2022,29 +2312,47 @@
         <v>1</v>
       </c>
       <c r="G33" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>7</v>
       </c>
       <c r="H33" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="I33" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>7</v>
       </c>
       <c r="J33" s="4" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>d</v>
+      </c>
+      <c r="K33">
+        <f t="shared" si="9"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:J33">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K33">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
half of implication table
</commit_message>
<xml_diff>
--- a/descreteMath/termpaper1/курсачтаблица.xlsx
+++ b/descreteMath/termpaper1/курсачтаблица.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\GitHub\ITMO-Labs\descreteMath\termpaper1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bernie\Documents\GitHub\ITMO-Labs\descreteMath\termpaper1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E4A1638-923E-44CE-BD8B-47EA95424380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4675E0-AFE1-42FD-A668-D0BA0F5D3C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2592" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="3405" windowWidth="13530" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -373,37 +373,7 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -436,116 +406,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -845,22 +705,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F17" sqref="B17:F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.88671875" customWidth="1"/>
-    <col min="2" max="6" width="3.33203125" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="6" width="3.28515625" customWidth="1"/>
     <col min="8" max="8" width="7" customWidth="1"/>
-    <col min="10" max="10" width="3.44140625" customWidth="1"/>
-    <col min="11" max="11" width="2.5546875" customWidth="1"/>
+    <col min="10" max="10" width="3.42578125" customWidth="1"/>
+    <col min="11" max="11" width="2.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -892,7 +752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>0</v>
       </c>
@@ -937,7 +797,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -982,7 +842,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -1027,7 +887,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1072,7 +932,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1117,7 +977,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1162,7 +1022,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1207,7 +1067,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1252,7 +1112,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1297,7 +1157,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1342,7 +1202,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1387,7 +1247,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1432,7 +1292,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1477,7 +1337,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1522,7 +1382,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1567,7 +1427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1612,7 +1472,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1657,7 +1517,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1702,7 +1562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1747,7 +1607,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1792,7 +1652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -1837,7 +1697,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -1882,7 +1742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -1927,7 +1787,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -1972,7 +1832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2017,7 +1877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2062,7 +1922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2107,7 +1967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -2152,7 +2012,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -2197,7 +2057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -2242,7 +2102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -2287,7 +2147,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2332,26 +2192,32 @@
         <v>5</v>
       </c>
     </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J34" s="4">
+        <f>COUNTIF(J2:J33, "=1")</f>
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="J2:J33">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+  <conditionalFormatting sqref="J2:J34">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K33">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>